<commit_message>
Assign to blocks - stage 1 (still to send the data via ajax)
</commit_message>
<xml_diff>
--- a/biasweb/data/output/ses-001-0042.xlsx
+++ b/biasweb/data/output/ses-001-0042.xlsx
@@ -1,20 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\biasweb.shazib\biasweb\data\output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="PD_ASSIGNED" sheetId="1" r:id="rId1"/>
+    <sheet name="Subjects" sheetId="1" r:id="rId1"/>
+    <sheet name="Pivot" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
+  <pivotCaches>
+    <pivotCache cacheId="4" r:id="rId3"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="70">
   <si>
     <t>ROLLNO</t>
   </si>
@@ -31,6 +40,9 @@
     <t>block_id</t>
   </si>
   <si>
+    <t>BATCHES</t>
+  </si>
+  <si>
     <t>16010002</t>
   </si>
   <si>
@@ -215,13 +227,19 @@
   </si>
   <si>
     <t>C120b</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of ROLLNO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,18 +291,603 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Dr. Shazib Ehsan" refreshedDate="43407.908277314818" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="48">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="B1:G49" sheet="Subjects"/>
+  </cacheSource>
+  <cacheFields count="6">
+    <cacheField name="ROLLNO" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="SECTION" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="EXP_CODE" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="block__serial_no" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="8" count="8">
+        <n v="8"/>
+        <n v="2"/>
+        <n v="5"/>
+        <n v="4"/>
+        <n v="7"/>
+        <n v="1"/>
+        <n v="3"/>
+        <n v="6"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="block_id" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="394" maxValue="401" count="8">
+        <n v="401"/>
+        <n v="395"/>
+        <n v="398"/>
+        <n v="397"/>
+        <n v="400"/>
+        <n v="394"/>
+        <n v="396"/>
+        <n v="399"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="BATCHES" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="3" count="3">
+        <n v="3"/>
+        <n v="2"/>
+        <n v="1"/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="48">
+  <r>
+    <s v="16010002"/>
+    <s v="A"/>
+    <s v="A012a"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010073"/>
+    <s v="A"/>
+    <s v="A012a"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010074"/>
+    <s v="A"/>
+    <s v="A012a"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010076"/>
+    <s v="A"/>
+    <s v="A012a"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010005"/>
+    <s v="A"/>
+    <s v="B012a"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010043"/>
+    <s v="A"/>
+    <s v="B012a"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010045"/>
+    <s v="A"/>
+    <s v="B012a"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010085"/>
+    <s v="B"/>
+    <s v="B012a"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010019"/>
+    <s v="A"/>
+    <s v="C012a"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010062"/>
+    <s v="B"/>
+    <s v="C012a"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010066"/>
+    <s v="A"/>
+    <s v="C012a"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010086"/>
+    <s v="B"/>
+    <s v="C012a"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010028"/>
+    <s v="A"/>
+    <s v="A012b"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010077"/>
+    <s v="B"/>
+    <s v="A012b"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010082"/>
+    <s v="B"/>
+    <s v="A012b"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010084"/>
+    <s v="A"/>
+    <s v="A012b"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010022"/>
+    <s v="B"/>
+    <s v="B012b"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010054"/>
+    <s v="A"/>
+    <s v="B012b"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010056"/>
+    <s v="A"/>
+    <s v="B012b"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010065"/>
+    <s v="B"/>
+    <s v="B012b"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010025"/>
+    <s v="B"/>
+    <s v="C012b"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010033"/>
+    <s v="A"/>
+    <s v="C012b"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010042"/>
+    <s v="B"/>
+    <s v="C012b"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010060"/>
+    <s v="A"/>
+    <s v="C012b"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010001"/>
+    <s v="A"/>
+    <s v="A120a"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010011"/>
+    <s v="A"/>
+    <s v="A120a"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010050"/>
+    <s v="B"/>
+    <s v="A120a"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010083"/>
+    <s v="B"/>
+    <s v="A120a"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010038"/>
+    <s v="A"/>
+    <s v="B120a"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010046"/>
+    <s v="B"/>
+    <s v="B120a"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010051"/>
+    <s v="B"/>
+    <s v="B120a"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010058"/>
+    <s v="A"/>
+    <s v="B120a"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010024"/>
+    <s v="B"/>
+    <s v="C120a"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010036"/>
+    <s v="B"/>
+    <s v="C120a"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010044"/>
+    <s v="A"/>
+    <s v="C120a"/>
+    <x v="1"/>
+    <x v="1"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010049"/>
+    <s v="A"/>
+    <s v="C120a"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010003"/>
+    <s v="A"/>
+    <s v="A120b"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010012"/>
+    <s v="A"/>
+    <s v="A120b"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010070"/>
+    <s v="B"/>
+    <s v="A120b"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010087"/>
+    <s v="B"/>
+    <s v="A120b"/>
+    <x v="0"/>
+    <x v="0"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010040"/>
+    <s v="A"/>
+    <s v="B120b"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <s v="16010047"/>
+    <s v="A"/>
+    <s v="B120b"/>
+    <x v="2"/>
+    <x v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010061"/>
+    <s v="A"/>
+    <s v="B120b"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010078"/>
+    <s v="A"/>
+    <s v="B120b"/>
+    <x v="3"/>
+    <x v="3"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010016"/>
+    <s v="A"/>
+    <s v="C120b"/>
+    <x v="5"/>
+    <x v="5"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010057"/>
+    <s v="A"/>
+    <s v="C120b"/>
+    <x v="7"/>
+    <x v="7"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <s v="16010064"/>
+    <s v="A"/>
+    <s v="C120b"/>
+    <x v="4"/>
+    <x v="4"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <s v="16010075"/>
+    <s v="A"/>
+    <s v="C120b"/>
+    <x v="6"/>
+    <x v="6"/>
+    <x v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+  <location ref="A3:E13" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="6">
+    <pivotField dataField="1" compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField compact="0" showAll="0"/>
+    <pivotField axis="axisRow" compact="0" showAll="0">
+      <items count="9">
+        <item x="5"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField compact="0" showAll="0">
+      <items count="9">
+        <item x="5"/>
+        <item x="1"/>
+        <item x="6"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="7"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" compact="0" showAll="0">
+      <items count="4">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="3"/>
+  </rowFields>
+  <rowItems count="9">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="5"/>
+  </colFields>
+  <colItems count="4">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of ROLLNO" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="1" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -330,7 +933,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -362,9 +965,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,6 +1000,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -571,14 +1176,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="15.21875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -594,99 +1204,114 @@
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6">
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F2">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>401</v>
+      </c>
+      <c r="G2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E3">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="F3">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>395</v>
+      </c>
+      <c r="G3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E4">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>395</v>
+      </c>
+      <c r="G4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="E5">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="F5">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>398</v>
+      </c>
+      <c r="G5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E6">
         <v>4</v>
@@ -694,339 +1319,390 @@
       <c r="F6">
         <v>397</v>
       </c>
-    </row>
-    <row r="7" spans="1:6">
+      <c r="G6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D7" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E7">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="F7">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>400</v>
+      </c>
+      <c r="G7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F8">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>397</v>
+      </c>
+      <c r="G8">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="E9">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F9">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>394</v>
+      </c>
+      <c r="G9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E10">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F10">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>401</v>
+      </c>
+      <c r="G10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D11" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E11">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+        <v>395</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E12">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+        <v>398</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="E13">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F13">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+        <v>398</v>
+      </c>
+      <c r="G13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D14" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E14">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F14">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+        <v>396</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C15" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D15" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E15">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F15">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+        <v>396</v>
+      </c>
+      <c r="G15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E16">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F16">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6">
+        <v>396</v>
+      </c>
+      <c r="G16">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D17" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E17">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="F17">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
+        <v>394</v>
+      </c>
+      <c r="G17">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D18" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E18">
+        <v>4</v>
+      </c>
+      <c r="F18">
+        <v>397</v>
+      </c>
+      <c r="G18">
         <v>1</v>
       </c>
-      <c r="F18">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E19">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="F19">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
+        <v>398</v>
+      </c>
+      <c r="G19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E20">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="F20">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6">
+        <v>397</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D21" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E21">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6">
+        <v>394</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D22" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E22">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F22">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6">
+        <v>395</v>
+      </c>
+      <c r="G22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C23" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D23" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E23">
         <v>8</v>
@@ -1034,99 +1710,114 @@
       <c r="F23">
         <v>401</v>
       </c>
-    </row>
-    <row r="24" spans="1:6">
+      <c r="G23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D24" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E24">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="F24">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6">
+        <v>399</v>
+      </c>
+      <c r="G24">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D25" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="E25">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="F25">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6">
+        <v>396</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D26" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="F26">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6">
+        <v>398</v>
+      </c>
+      <c r="G26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D27" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E27">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="F27">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6">
+        <v>401</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E28">
         <v>8</v>
@@ -1134,139 +1825,160 @@
       <c r="F28">
         <v>401</v>
       </c>
-    </row>
-    <row r="29" spans="1:6">
+      <c r="G28">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C29" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D29" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="E29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F29">
-        <v>401</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6">
+        <v>400</v>
+      </c>
+      <c r="G29">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C30" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E30">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="F30">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6">
+        <v>400</v>
+      </c>
+      <c r="G30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="C31" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D31" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E31">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="F31">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6">
+        <v>395</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C32" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D32" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F32">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6">
+        <v>394</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D33" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="E33">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="F33">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6">
+        <v>399</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C34" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E34">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="F34">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6">
+        <v>397</v>
+      </c>
+      <c r="G34">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C35" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E35">
         <v>6</v>
@@ -1274,59 +1986,68 @@
       <c r="F35">
         <v>399</v>
       </c>
-    </row>
-    <row r="36" spans="1:6">
+      <c r="G35">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E36">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F36">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6">
+        <v>395</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C37" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="E37">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F37">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6">
+        <v>399</v>
+      </c>
+      <c r="G37">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C38" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D38" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E38">
         <v>6</v>
@@ -1334,19 +2055,22 @@
       <c r="F38">
         <v>399</v>
       </c>
-    </row>
-    <row r="39" spans="1:6">
+      <c r="G38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D39" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E39">
         <v>7</v>
@@ -1354,19 +2078,22 @@
       <c r="F39">
         <v>400</v>
       </c>
-    </row>
-    <row r="40" spans="1:6">
+      <c r="G39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C40" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D40" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E40">
         <v>7</v>
@@ -1374,39 +2101,45 @@
       <c r="F40">
         <v>400</v>
       </c>
-    </row>
-    <row r="41" spans="1:6">
+      <c r="G40">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C41" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D41" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="E41">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="F41">
-        <v>396</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6">
+        <v>401</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C42" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D42" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E42">
         <v>1</v>
@@ -1414,99 +2147,114 @@
       <c r="F42">
         <v>394</v>
       </c>
-    </row>
-    <row r="43" spans="1:6">
+      <c r="G42">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D43" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E43">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F43">
-        <v>397</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6">
+        <v>398</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C44" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D44" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E44">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F44">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6">
+        <v>396</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C45" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D45" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="E45">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F45">
-        <v>399</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6">
+        <v>397</v>
+      </c>
+      <c r="G45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C46" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D46" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E46">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F46">
-        <v>398</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6">
+        <v>394</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C47" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D47" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E47">
         <v>6</v>
@@ -1514,45 +2262,254 @@
       <c r="F47">
         <v>399</v>
       </c>
-    </row>
-    <row r="48" spans="1:6">
+      <c r="G47">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D48" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E48">
+        <v>7</v>
+      </c>
+      <c r="F48">
+        <v>400</v>
+      </c>
+      <c r="G48">
         <v>1</v>
       </c>
-      <c r="F48">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6">
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C49" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D49" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="E49">
+        <v>3</v>
+      </c>
+      <c r="F49">
+        <v>396</v>
+      </c>
+      <c r="G49">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="4" width="10.88671875" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="6" max="8" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F49">
-        <v>398</v>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>3</v>
+      </c>
+      <c r="E4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" s="3">
+        <v>2</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>4</v>
+      </c>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>6</v>
+      </c>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3">
+        <v>2</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>2</v>
+      </c>
+      <c r="E11" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>8</v>
+      </c>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2</v>
+      </c>
+      <c r="E12" s="3">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="3">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3">
+        <v>16</v>
+      </c>
+      <c r="D13" s="3">
+        <v>16</v>
+      </c>
+      <c r="E13" s="3">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>